<commit_message>
color change foothold material, ev, tu light cpp
</commit_message>
<xml_diff>
--- a/계획표.xlsx
+++ b/계획표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dounii\Desktop\TCM\TCM_Cobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA4118A-7C5F-46F8-8C41-821028B327B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F57304-1C81-4936-A60F-7EEC7ACCBA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" xr2:uid="{B06EFC80-A5D2-40DD-894D-9DDAD4D977BC}"/>
+    <workbookView xWindow="2630" yWindow="2630" windowWidth="18031" windowHeight="9303" xr2:uid="{B06EFC80-A5D2-40DD-894D-9DDAD4D977BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
   <si>
     <t>01.16 ~ 01.22</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1067,6 +1067,10 @@
   </si>
   <si>
     <t>시네마틱 완성 // ppt 제작 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt -&gt; 1장. 기획서 바뀐거 / 2장. 진행상황</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1496,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E8A85B-B798-4185-9BD1-C35E8FAE44D2}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.2" x14ac:dyDescent="0.4"/>
@@ -1868,6 +1872,9 @@
       <c r="B38" t="s">
         <v>80</v>
       </c>
+      <c r="D38" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" t="s">

</xml_diff>